<commit_message>
Commit for updating runtime summary metrics spreadsheet with latest data.
</commit_message>
<xml_diff>
--- a/metrics_data/runtime_summary_20251205_071834.xlsx
+++ b/metrics_data/runtime_summary_20251205_071834.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dennyr\Dropbox\Education\Southern Methodist University\Courses\Software Architecture &amp; Design CS7319\Project\musicbrainz-app\metrics_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{26FA7817-6E31-4266-95FA-11338FFD9777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F5F7C1-09D2-4C42-A018-A73E1F8A7A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{662A5ED0-39A7-4C70-8BF2-A6D310E7FE8B}"/>
   </bookViews>
@@ -6692,21 +6692,22 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="0" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="22.5703125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="32.28515625" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="20.5703125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>